<commit_message>
spring 2020 data added
</commit_message>
<xml_diff>
--- a/GroupsandSubgroups.xlsx
+++ b/GroupsandSubgroups.xlsx
@@ -58,16 +58,16 @@
     <t xml:space="preserve">CHY1</t>
   </si>
   <si>
-    <t xml:space="preserve">CSE1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSE11(32),CSE12(32),CSE13(32),CSE14(31)</t>
+    <t xml:space="preserve">CSD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSD11(35),CSD12(34),CSD13(34)</t>
   </si>
   <si>
     <t xml:space="preserve">ECE1</t>
   </si>
   <si>
-    <t xml:space="preserve">ECE11(30),ECE12(30),ECE13(22)</t>
+    <t xml:space="preserve">ECE11(30),ECE12(24)</t>
   </si>
   <si>
     <t xml:space="preserve">ECO1</t>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">EEE1</t>
   </si>
   <si>
-    <t xml:space="preserve">EEE11(30),EEE12(29)</t>
+    <t xml:space="preserve">EEE11(30),EEE12(11)</t>
   </si>
   <si>
     <t xml:space="preserve">ENG1</t>
@@ -94,7 +94,7 @@
     <t xml:space="preserve">MED1</t>
   </si>
   <si>
-    <t xml:space="preserve">MED11(29),MED12(28)</t>
+    <t xml:space="preserve">MED11(30),MED12(10)</t>
   </si>
   <si>
     <t xml:space="preserve">PHY1</t>
@@ -118,10 +118,10 @@
     <t xml:space="preserve">CHY2</t>
   </si>
   <si>
-    <t xml:space="preserve">CSE2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSE21(30),CSE22(17)</t>
+    <t xml:space="preserve">CSD2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSD21(30),CSD22(17)</t>
   </si>
   <si>
     <t xml:space="preserve">ECE2</t>
@@ -172,10 +172,10 @@
     <t xml:space="preserve">CHY3</t>
   </si>
   <si>
-    <t xml:space="preserve">CSE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSE31(29),CSE32(28)</t>
+    <t xml:space="preserve">CSD3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSD31(29),CSD32(28)</t>
   </si>
   <si>
     <t xml:space="preserve">ECE3</t>
@@ -229,7 +229,7 @@
     <t xml:space="preserve">CHY4</t>
   </si>
   <si>
-    <t xml:space="preserve">CSE4</t>
+    <t xml:space="preserve">CSD4</t>
   </si>
   <si>
     <t xml:space="preserve">ECE4</t>
@@ -382,8 +382,8 @@
   </sheetPr>
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -475,7 +475,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
@@ -503,7 +503,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
@@ -520,7 +520,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -551,7 +551,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>17</v>
@@ -624,7 +624,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>23</v>

</xml_diff>